<commit_message>
Add and update pandas demos.
</commit_message>
<xml_diff>
--- a/pydemos/data/lemon_cases.xlsx
+++ b/pydemos/data/lemon_cases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengjin/Workspaces/zj_py3_project/pydemos/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5D26A5CD-599C-CA42-8878-D9D42AF5BA83}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F46A06D2-CF5A-0949-A44C-0D09DE88DF91}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{3D469D55-1862-E347-A8A7-0C21055D17AF}"/>
   </bookViews>
   <sheets>
-    <sheet name="multiply" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="multiply" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>case_id</t>
   </si>
@@ -64,16 +65,108 @@
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>name2</t>
+  </si>
+  <si>
+    <t>name3</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>mail1@gmail.com</t>
+  </si>
+  <si>
+    <t>mail2@163.com</t>
+  </si>
+  <si>
+    <t>mail3@qq.com</t>
+  </si>
+  <si>
+    <t>name4</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>1991-11-01</t>
+  </si>
+  <si>
+    <t>1990-05-25</t>
+  </si>
+  <si>
+    <t>1992-02-16</t>
+  </si>
+  <si>
+    <t>2010-09-10</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>name5</t>
+  </si>
+  <si>
+    <t>name6</t>
+  </si>
+  <si>
+    <t>mail5@gmail.com</t>
+  </si>
+  <si>
+    <t>mail4@gmail.com</t>
+  </si>
+  <si>
+    <t>mail6@163.com</t>
+  </si>
+  <si>
+    <t>1885-01-13</t>
+  </si>
+  <si>
+    <t>1990-12-01</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,16 +189,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,10 +515,194 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88660CAB-7CE6-9E40-8936-B8CDB8616AF1}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4">
+        <v>12000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4">
+        <v>11000</v>
+      </c>
+      <c r="F3" s="4">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4">
+        <v>9000</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="4">
+        <v>22000</v>
+      </c>
+      <c r="F5" s="4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="4">
+        <v>21000</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B7DB3309-899C-0A45-949C-FB2C26E90F4D}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{290C1FA5-0F22-4942-BB9D-AA8E03FE41E8}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{DCD500A7-7B42-9F4E-B039-71764BFBF618}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{426700DD-1A56-D04F-B3D4-BC3B6CB6E828}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{34179B92-D993-534E-A728-2459DEFDE983}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{5D91E515-A6DC-F045-A833-14AF98876DCF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FAA268-B4B5-3947-AEF9-749BE5CA7C85}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>